<commit_message>
Implemented Array Questions test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\eclipse-workspace\DsAlgo-Testng\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SeleniumTestNG\DsAlgo_Testng\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4D7A3E-F00F-4D97-A3DF-50EE5FF21AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3280F63A-0483-48B0-AC74-880CE097F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-170" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="7" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>Find Numbers with Even Number of Digits</t>
   </si>
   <si>
-    <t>Squares of a Sorted Array</t>
-  </si>
-  <si>
     <t>sdet86batch1</t>
   </si>
   <si>
@@ -221,17 +218,27 @@
   </si>
   <si>
     <t>password_invalid</t>
+  </si>
+  <si>
+    <t>Squares of  a Sorted Array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,21 +305,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,14 +543,14 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,18 +561,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,7 +583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,12 +594,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -609,21 +617,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="30.21875" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -631,80 +639,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -724,12 +732,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -737,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -745,7 +753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -766,16 +774,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -786,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -797,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -808,7 +816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -819,9 +827,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -843,16 +851,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.88671875" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -863,7 +871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -874,7 +882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -885,7 +893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -896,9 +904,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -919,18 +927,18 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -941,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -952,7 +960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -963,7 +971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -974,9 +982,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -986,7 +994,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Login Page Tests and added Listeners to all page tests for ExtentReport generation
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\git\DsAlgo_Testng\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SeleniumTestNG\DsAlgo_Testng\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F488CF8-4E73-43E4-AA0F-E059DF1A2334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A612D264-D861-4567-93CA-E894FA63A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -142,12 +142,6 @@
     <t>[4, 9, 9, 49, 121]</t>
   </si>
   <si>
-    <t>Please check your user id</t>
-  </si>
-  <si>
-    <t>Please check your password</t>
-  </si>
-  <si>
     <t>NameError: name 'hello' is not defined on line 1</t>
   </si>
   <si>
@@ -224,6 +218,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>pwd1234</t>
+  </si>
+  <si>
+    <t>invalid_data</t>
+  </si>
+  <si>
+    <t>valid_data</t>
   </si>
 </sst>
 </file>
@@ -540,20 +543,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD3EF51-3903-43CC-AD16-52D599F2FE39}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,49 +567,98 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -620,21 +673,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,98 +695,98 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -753,12 +806,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -766,7 +819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -774,12 +827,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -798,15 +851,15 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -815,9 +868,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -826,9 +879,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
@@ -837,9 +890,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -848,9 +901,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -875,15 +928,15 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.88671875" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -892,9 +945,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -903,9 +956,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
@@ -914,9 +967,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -925,9 +978,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -952,16 +1005,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -970,48 +1023,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dataprovider -put invalid and valid data in separate sheets for scalability
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,27 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SeleniumTestNG\DsAlgo_Testng\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\git\DsAlgo_Testng\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A612D264-D861-4567-93CA-E894FA63A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA3B47-C0F1-4D52-A447-0CC5C6573CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginSheet" sheetId="7" r:id="rId1"/>
-    <sheet name="registrationSheet" sheetId="1" r:id="rId2"/>
-    <sheet name="pythonCode" sheetId="2" r:id="rId3"/>
-    <sheet name="validPythonCode" sheetId="3" r:id="rId4"/>
-    <sheet name="submitPythonCode" sheetId="4" r:id="rId5"/>
-    <sheet name="invalidPythonCode" sheetId="6" r:id="rId6"/>
+    <sheet name="validLoginSheet" sheetId="8" r:id="rId1"/>
+    <sheet name="invalidLoginSheet" sheetId="7" r:id="rId2"/>
+    <sheet name="registrationSheet" sheetId="1" r:id="rId3"/>
+    <sheet name="validTryEditor" sheetId="2" r:id="rId4"/>
+    <sheet name="invalidTryEditor" sheetId="9" r:id="rId5"/>
+    <sheet name="validPythonCode" sheetId="3" r:id="rId6"/>
+    <sheet name="submitPythonCode" sheetId="4" r:id="rId7"/>
+    <sheet name="invalidPythonCode" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -542,22 +544,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD3EF51-3903-43CC-AD16-52D599F2FE39}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E16AB4-407E-4D97-B845-E9C0F5B52B99}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +573,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
@@ -585,109 +587,144 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{57D8A557-E7A5-4C4D-86F5-F523C4AA7ABF}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3094E4A1-D04A-4CF7-91AF-350F212D9BB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD3EF51-3903-43CC-AD16-52D599F2FE39}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" customWidth="1"/>
+    <col min="6" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +741,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -721,7 +758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -738,7 +775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -755,7 +792,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -772,7 +809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -795,23 +832,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -819,20 +856,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +869,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCB044B-6BEB-4771-B662-1AF37E1834E9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA999A81-B0C1-4E69-8277-B2FB3354048F}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -851,13 +914,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -868,7 +931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -879,7 +942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -890,7 +953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -901,7 +964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -917,7 +980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AE293B-0379-4C23-BB59-06FA968BFA5A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -928,13 +991,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.85546875" customWidth="1"/>
+    <col min="2" max="2" width="118.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -945,7 +1008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -956,7 +1019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -967,7 +1030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -978,7 +1041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>45</v>
       </c>
@@ -994,7 +1057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE603DDD-C237-4E6E-9DD6-17BAB081D59A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1005,14 +1068,14 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1023,7 +1086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1034,7 +1097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1045,7 +1108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1056,7 +1119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>

</xml_diff>